<commit_message>
update for day 3
</commit_message>
<xml_diff>
--- a/Tournament1BracketWorking.xlsx
+++ b/Tournament1BracketWorking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apache24\htdocs\Databse-Project-TBD\TheShowdownEffect.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1E32D3-2847-4258-8F86-4ECB8751D269}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3DDB8A-7BD8-44B9-A0F8-399D61FBE2D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10035" yWindow="4800" windowWidth="25485" windowHeight="14595" xr2:uid="{D7CBCFDF-C382-44AA-938F-833AB08825E4}"/>
+    <workbookView xWindow="12210" yWindow="4275" windowWidth="25485" windowHeight="14595" xr2:uid="{D7CBCFDF-C382-44AA-938F-833AB08825E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,36 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
-  <si>
-    <t>Team 2</t>
-  </si>
-  <si>
-    <t>Loser of 8</t>
-  </si>
-  <si>
-    <t>Loser of 7</t>
-  </si>
-  <si>
-    <t>Loser of 12</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>Champion</t>
   </si>
   <si>
     <t>Showdown Effect Tournament</t>
-  </si>
-  <si>
-    <t>Loser of 5</t>
-  </si>
-  <si>
-    <t>Loser of 6</t>
-  </si>
-  <si>
-    <t>Loser of 9</t>
-  </si>
-  <si>
-    <t>Loser of 10</t>
   </si>
   <si>
     <t>Match 1</t>
@@ -123,12 +99,6 @@
     <t>Match 13 (Loser is 7th Place)</t>
   </si>
   <si>
-    <t>Loser of 14</t>
-  </si>
-  <si>
-    <t>Loser of 19 (If only one loss)</t>
-  </si>
-  <si>
     <t>Match 15</t>
   </si>
   <si>
@@ -153,7 +123,49 @@
     <t>Forgot to Warm Up</t>
   </si>
   <si>
-    <t>Loser of 15</t>
+    <t>2 Bacon Nuggets</t>
+  </si>
+  <si>
+    <t>Loser of Match 1</t>
+  </si>
+  <si>
+    <t>Loser of Match 2</t>
+  </si>
+  <si>
+    <t>Loser of Match 3</t>
+  </si>
+  <si>
+    <t>Loser of Match 4</t>
+  </si>
+  <si>
+    <t>Loser of Match 8</t>
+  </si>
+  <si>
+    <t>Loser of Match 7</t>
+  </si>
+  <si>
+    <t>Loser of Match 12</t>
+  </si>
+  <si>
+    <t>Loser of Match 14</t>
+  </si>
+  <si>
+    <t>Loser of Match 15</t>
+  </si>
+  <si>
+    <t>Loser of Match 19 (If one loss)</t>
+  </si>
+  <si>
+    <t>Loser of Match 5</t>
+  </si>
+  <si>
+    <t>Loser of Match 6</t>
+  </si>
+  <si>
+    <t>Loser of Match 9</t>
+  </si>
+  <si>
+    <t>Loser of Match 10</t>
   </si>
 </sst>
 </file>
@@ -301,15 +313,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -319,8 +322,17 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3509,8 +3521,8 @@
   </sheetPr>
   <dimension ref="C2:T63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3537,21 +3549,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:20" ht="35.25">
-      <c r="C2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
+      <c r="C2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="3:20">
@@ -3585,12 +3597,12 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="Q4" s="8"/>
-      <c r="R4" s="11"/>
+      <c r="R4" s="14"/>
       <c r="T4" s="8"/>
     </row>
     <row r="5" spans="3:20">
       <c r="C5" s="4" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -3605,16 +3617,16 @@
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
       <c r="Q5" s="8"/>
-      <c r="R5" s="11"/>
+      <c r="R5" s="14"/>
       <c r="T5" s="8"/>
     </row>
     <row r="6" spans="3:20">
       <c r="C6" s="5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="4" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -3627,12 +3639,12 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="Q6" s="8"/>
-      <c r="R6" s="11"/>
+      <c r="R6" s="14"/>
       <c r="T6" s="8"/>
     </row>
     <row r="7" spans="3:20">
       <c r="C7" s="4" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -3647,7 +3659,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="Q7" s="8"/>
-      <c r="R7" s="11"/>
+      <c r="R7" s="14"/>
       <c r="T7" s="8"/>
     </row>
     <row r="8" spans="3:20">
@@ -3665,17 +3677,19 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="Q8" s="8"/>
-      <c r="R8" s="11"/>
+      <c r="R8" s="14"/>
       <c r="T8" s="8"/>
     </row>
     <row r="9" spans="3:20">
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="6" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F9" s="5"/>
-      <c r="G9" s="4"/>
+      <c r="G9" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -3685,7 +3699,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="Q9" s="8"/>
-      <c r="R9" s="11"/>
+      <c r="R9" s="14"/>
       <c r="T9" s="8"/>
     </row>
     <row r="10" spans="3:20">
@@ -3703,12 +3717,12 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="Q10" s="8"/>
-      <c r="R10" s="11"/>
+      <c r="R10" s="14"/>
       <c r="T10" s="8"/>
     </row>
     <row r="11" spans="3:20">
       <c r="C11" s="4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -3723,16 +3737,16 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="Q11" s="8"/>
-      <c r="R11" s="11"/>
+      <c r="R11" s="14"/>
       <c r="T11" s="8"/>
     </row>
     <row r="12" spans="3:20">
       <c r="C12" s="5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -3745,12 +3759,12 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="Q12" s="8"/>
-      <c r="R12" s="11"/>
+      <c r="R12" s="14"/>
       <c r="T12" s="8"/>
     </row>
     <row r="13" spans="3:20">
       <c r="C13" s="4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -3765,7 +3779,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="Q13" s="8"/>
-      <c r="R13" s="11"/>
+      <c r="R13" s="14"/>
       <c r="T13" s="8"/>
     </row>
     <row r="14" spans="3:20">
@@ -3783,7 +3797,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="Q14" s="8"/>
-      <c r="R14" s="11"/>
+      <c r="R14" s="14"/>
       <c r="T14" s="8"/>
     </row>
     <row r="15" spans="3:20">
@@ -3792,18 +3806,18 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="6" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="H15" s="5"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="14"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="11"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="Q15" s="8"/>
-      <c r="R15" s="11"/>
+      <c r="R15" s="14"/>
       <c r="T15" s="8"/>
     </row>
     <row r="16" spans="3:20">
@@ -3821,12 +3835,12 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="Q16" s="8"/>
-      <c r="R16" s="11"/>
+      <c r="R16" s="14"/>
       <c r="T16" s="8"/>
     </row>
     <row r="17" spans="3:20">
       <c r="C17" s="4" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -3841,16 +3855,16 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="Q17" s="8"/>
-      <c r="R17" s="11"/>
+      <c r="R17" s="14"/>
       <c r="T17" s="8"/>
     </row>
     <row r="18" spans="3:20">
       <c r="C18" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -3863,12 +3877,12 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="Q18" s="8"/>
-      <c r="R18" s="11"/>
+      <c r="R18" s="14"/>
       <c r="T18" s="8"/>
     </row>
     <row r="19" spans="3:20">
       <c r="C19" s="4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -3883,7 +3897,7 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="Q19" s="8"/>
-      <c r="R19" s="11"/>
+      <c r="R19" s="14"/>
       <c r="T19" s="8"/>
     </row>
     <row r="20" spans="3:20">
@@ -3901,17 +3915,19 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="Q20" s="8"/>
-      <c r="R20" s="11"/>
+      <c r="R20" s="14"/>
       <c r="T20" s="8"/>
     </row>
     <row r="21" spans="3:20">
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="6" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F21" s="5"/>
-      <c r="G21" s="4"/>
+      <c r="G21" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
@@ -3921,7 +3937,7 @@
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="Q21" s="8"/>
-      <c r="R21" s="11"/>
+      <c r="R21" s="14"/>
       <c r="T21" s="8"/>
     </row>
     <row r="22" spans="3:20">
@@ -3939,12 +3955,12 @@
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="Q22" s="8"/>
-      <c r="R22" s="11"/>
+      <c r="R22" s="14"/>
       <c r="T22" s="8"/>
     </row>
     <row r="23" spans="3:20">
       <c r="C23" s="4" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -3955,20 +3971,22 @@
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
+      <c r="M23" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
       <c r="Q23" s="8"/>
-      <c r="R23" s="11"/>
+      <c r="R23" s="14"/>
       <c r="T23" s="8"/>
     </row>
     <row r="24" spans="3:20">
       <c r="C24" s="5" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -3977,18 +3995,16 @@
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
-      <c r="M24" s="4" t="s">
-        <v>30</v>
-      </c>
+      <c r="M24" s="4"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
       <c r="Q24" s="8"/>
-      <c r="R24" s="11"/>
+      <c r="R24" s="14"/>
       <c r="T24" s="8"/>
     </row>
     <row r="25" spans="3:20">
       <c r="C25" s="4" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
@@ -4000,14 +4016,14 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="N25" s="5"/>
       <c r="O25" s="4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q25" s="8"/>
-      <c r="R25" s="11"/>
+      <c r="R25" s="14"/>
       <c r="T25" s="8"/>
     </row>
     <row r="26" spans="3:20">
@@ -4016,18 +4032,18 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
+      <c r="H26" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
       <c r="L26" s="5"/>
       <c r="M26" s="4"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
       <c r="Q26" s="8"/>
-      <c r="R26" s="11"/>
+      <c r="R26" s="14"/>
       <c r="T26" s="8"/>
     </row>
     <row r="27" spans="3:20">
@@ -4045,7 +4061,7 @@
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
       <c r="Q27" s="8"/>
-      <c r="R27" s="11"/>
+      <c r="R27" s="14"/>
       <c r="T27" s="8"/>
     </row>
     <row r="28" spans="3:20">
@@ -4063,7 +4079,7 @@
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
       <c r="Q28" s="8"/>
-      <c r="R28" s="11"/>
+      <c r="R28" s="14"/>
       <c r="T28" s="8"/>
     </row>
     <row r="29" spans="3:20">
@@ -4081,7 +4097,7 @@
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
       <c r="Q29" s="8"/>
-      <c r="R29" s="11"/>
+      <c r="R29" s="14"/>
       <c r="T29" s="8"/>
     </row>
     <row r="30" spans="3:20">
@@ -4099,7 +4115,7 @@
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="Q30" s="8"/>
-      <c r="R30" s="11"/>
+      <c r="R30" s="14"/>
       <c r="T30" s="8"/>
     </row>
     <row r="31" spans="3:20">
@@ -4117,7 +4133,7 @@
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="Q31" s="8"/>
-      <c r="R31" s="11"/>
+      <c r="R31" s="14"/>
       <c r="T31" s="8"/>
     </row>
     <row r="32" spans="3:20">
@@ -4135,13 +4151,15 @@
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
       <c r="Q32" s="8"/>
-      <c r="R32" s="11"/>
+      <c r="R32" s="14"/>
       <c r="T32" s="8"/>
     </row>
     <row r="33" spans="3:20">
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
+      <c r="E33" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
@@ -4153,14 +4171,16 @@
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="Q33" s="8"/>
-      <c r="R33" s="11"/>
+      <c r="R33" s="14"/>
       <c r="T33" s="8"/>
     </row>
     <row r="34" spans="3:20">
-      <c r="C34" s="7"/>
+      <c r="C34" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="D34" s="5"/>
       <c r="E34" s="4" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
@@ -4173,19 +4193,21 @@
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
       <c r="Q34" s="8"/>
-      <c r="R34" s="11"/>
+      <c r="R34" s="14"/>
       <c r="T34" s="8"/>
     </row>
     <row r="35" spans="3:20">
       <c r="C35" s="4" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="6" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F35" s="5"/>
-      <c r="G35" s="4"/>
+      <c r="G35" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
@@ -4195,19 +4217,23 @@
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
       <c r="Q35" s="8"/>
-      <c r="R35" s="11"/>
+      <c r="R35" s="14"/>
       <c r="T35" s="8"/>
     </row>
     <row r="36" spans="3:20">
       <c r="C36" s="5" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D36" s="5"/>
-      <c r="E36" s="4"/>
+      <c r="E36" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
+      <c r="I36" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
@@ -4217,16 +4243,14 @@
     </row>
     <row r="37" spans="3:20">
       <c r="C37" s="4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
-      <c r="I37" s="4" t="s">
-        <v>39</v>
-      </c>
+      <c r="I37" s="4"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
@@ -4235,14 +4259,16 @@
       <c r="O37" s="5"/>
     </row>
     <row r="38" spans="3:20">
-      <c r="C38" s="5"/>
+      <c r="C38" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="J38" s="5"/>
       <c r="K38" s="4"/>
@@ -4250,9 +4276,9 @@
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
-      <c r="R38" s="9"/>
-      <c r="S38" s="9"/>
-      <c r="T38" s="9"/>
+      <c r="R38" s="15"/>
+      <c r="S38" s="15"/>
+      <c r="T38" s="15"/>
     </row>
     <row r="39" spans="3:20">
       <c r="C39" s="5"/>
@@ -4260,7 +4286,7 @@
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="6" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="4"/>
@@ -4270,12 +4296,14 @@
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
-      <c r="R39" s="9"/>
-      <c r="S39" s="9"/>
-      <c r="T39" s="9"/>
+      <c r="R39" s="15"/>
+      <c r="S39" s="15"/>
+      <c r="T39" s="15"/>
     </row>
     <row r="40" spans="3:20">
-      <c r="C40" s="5"/>
+      <c r="C40" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
@@ -4291,7 +4319,7 @@
     </row>
     <row r="41" spans="3:20">
       <c r="C41" s="4" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
@@ -4308,10 +4336,12 @@
     </row>
     <row r="42" spans="3:20">
       <c r="C42" s="5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D42" s="5"/>
-      <c r="E42" s="4"/>
+      <c r="E42" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
@@ -4325,14 +4355,16 @@
     </row>
     <row r="43" spans="3:20">
       <c r="C43" s="4" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F43" s="5"/>
-      <c r="G43" s="4"/>
+      <c r="G43" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
@@ -4343,10 +4375,12 @@
       <c r="O43" s="5"/>
     </row>
     <row r="44" spans="3:20">
-      <c r="C44" s="5"/>
+      <c r="C44" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
@@ -4362,7 +4396,9 @@
     <row r="45" spans="3:20">
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
+      <c r="E45" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
@@ -4452,7 +4488,9 @@
     <row r="51" spans="3:15">
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
+      <c r="E51" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
@@ -4465,11 +4503,11 @@
       <c r="O51" s="5"/>
     </row>
     <row r="52" spans="3:15">
-      <c r="C52" s="5"/>
+      <c r="C52" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="D52" s="5"/>
-      <c r="E52" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="E52" s="4"/>
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
@@ -4483,11 +4521,11 @@
     </row>
     <row r="53" spans="3:15">
       <c r="C53" s="4" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F53" s="5"/>
       <c r="G53" s="4"/>
@@ -4502,14 +4540,16 @@
     </row>
     <row r="54" spans="3:15">
       <c r="C54" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="4"/>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
+      <c r="I54" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
@@ -4519,16 +4559,14 @@
     </row>
     <row r="55" spans="3:15">
       <c r="C55" s="4" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
-      <c r="I55" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="I55" s="4"/>
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
@@ -4537,14 +4575,16 @@
       <c r="O55" s="5"/>
     </row>
     <row r="56" spans="3:15">
-      <c r="C56" s="5"/>
+      <c r="C56" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
       <c r="I56" s="6" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="J56" s="5"/>
       <c r="K56" s="4"/>
@@ -4556,11 +4596,11 @@
     <row r="57" spans="3:15">
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
-      <c r="E57" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F57" s="10"/>
-      <c r="G57" s="10"/>
+      <c r="E57" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
       <c r="H57" s="5"/>
       <c r="I57" s="4"/>
       <c r="J57" s="5"/>
@@ -4586,7 +4626,9 @@
       <c r="O58" s="5"/>
     </row>
     <row r="59" spans="3:15">
-      <c r="C59" s="5"/>
+      <c r="C59" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
@@ -4602,7 +4644,7 @@
     </row>
     <row r="60" spans="3:15">
       <c r="C60" s="4" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
@@ -4619,12 +4661,12 @@
     </row>
     <row r="61" spans="3:15">
       <c r="C61" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D61" s="5"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="13"/>
-      <c r="G61" s="14"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="11"/>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
@@ -4636,7 +4678,7 @@
     </row>
     <row r="62" spans="3:15">
       <c r="C62" s="4" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
@@ -4652,7 +4694,9 @@
       <c r="O62" s="5"/>
     </row>
     <row r="63" spans="3:15">
-      <c r="C63" s="5"/>
+      <c r="C63" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
@@ -4668,11 +4712,16 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="Q24:Q27"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="C2:O2"/>
+    <mergeCell ref="T28:T31"/>
+    <mergeCell ref="T32:T35"/>
+    <mergeCell ref="R38:T38"/>
+    <mergeCell ref="R39:T39"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="T4:T7"/>
+    <mergeCell ref="T8:T11"/>
+    <mergeCell ref="T12:T15"/>
+    <mergeCell ref="T16:T19"/>
+    <mergeCell ref="T20:T23"/>
     <mergeCell ref="T24:T27"/>
     <mergeCell ref="Q28:Q31"/>
     <mergeCell ref="Q32:Q35"/>
@@ -4689,16 +4738,11 @@
     <mergeCell ref="Q12:Q15"/>
     <mergeCell ref="Q16:Q19"/>
     <mergeCell ref="Q20:Q23"/>
-    <mergeCell ref="T4:T7"/>
-    <mergeCell ref="T8:T11"/>
-    <mergeCell ref="T12:T15"/>
-    <mergeCell ref="T16:T19"/>
-    <mergeCell ref="T20:T23"/>
-    <mergeCell ref="T28:T31"/>
-    <mergeCell ref="T32:T35"/>
-    <mergeCell ref="R38:T38"/>
-    <mergeCell ref="R39:T39"/>
-    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="Q24:Q27"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="C2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
end of day 3 update p2
</commit_message>
<xml_diff>
--- a/Tournament1BracketWorking.xlsx
+++ b/Tournament1BracketWorking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apache24\htdocs\Databse-Project-TBD\TheShowdownEffect.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3DDB8A-7BD8-44B9-A0F8-399D61FBE2D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E381DE-805A-45CC-B52A-842B48AF5F1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12210" yWindow="4275" windowWidth="25485" windowHeight="14595" xr2:uid="{D7CBCFDF-C382-44AA-938F-833AB08825E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D7CBCFDF-C382-44AA-938F-833AB08825E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>Champion</t>
   </si>
@@ -313,6 +313,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -322,17 +331,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3521,8 +3521,8 @@
   </sheetPr>
   <dimension ref="C2:T63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V28" sqref="V28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3549,21 +3549,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:20" ht="35.25">
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="3:20">
@@ -3597,7 +3597,7 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="Q4" s="8"/>
-      <c r="R4" s="14"/>
+      <c r="R4" s="11"/>
       <c r="T4" s="8"/>
     </row>
     <row r="5" spans="3:20">
@@ -3617,7 +3617,7 @@
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
       <c r="Q5" s="8"/>
-      <c r="R5" s="14"/>
+      <c r="R5" s="11"/>
       <c r="T5" s="8"/>
     </row>
     <row r="6" spans="3:20">
@@ -3639,7 +3639,7 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="Q6" s="8"/>
-      <c r="R6" s="14"/>
+      <c r="R6" s="11"/>
       <c r="T6" s="8"/>
     </row>
     <row r="7" spans="3:20">
@@ -3659,7 +3659,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="Q7" s="8"/>
-      <c r="R7" s="14"/>
+      <c r="R7" s="11"/>
       <c r="T7" s="8"/>
     </row>
     <row r="8" spans="3:20">
@@ -3677,7 +3677,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="Q8" s="8"/>
-      <c r="R8" s="14"/>
+      <c r="R8" s="11"/>
       <c r="T8" s="8"/>
     </row>
     <row r="9" spans="3:20">
@@ -3699,7 +3699,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="Q9" s="8"/>
-      <c r="R9" s="14"/>
+      <c r="R9" s="11"/>
       <c r="T9" s="8"/>
     </row>
     <row r="10" spans="3:20">
@@ -3717,7 +3717,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="Q10" s="8"/>
-      <c r="R10" s="14"/>
+      <c r="R10" s="11"/>
       <c r="T10" s="8"/>
     </row>
     <row r="11" spans="3:20">
@@ -3737,7 +3737,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="Q11" s="8"/>
-      <c r="R11" s="14"/>
+      <c r="R11" s="11"/>
       <c r="T11" s="8"/>
     </row>
     <row r="12" spans="3:20">
@@ -3759,7 +3759,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="Q12" s="8"/>
-      <c r="R12" s="14"/>
+      <c r="R12" s="11"/>
       <c r="T12" s="8"/>
     </row>
     <row r="13" spans="3:20">
@@ -3779,7 +3779,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="Q13" s="8"/>
-      <c r="R13" s="14"/>
+      <c r="R13" s="11"/>
       <c r="T13" s="8"/>
     </row>
     <row r="14" spans="3:20">
@@ -3797,7 +3797,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="Q14" s="8"/>
-      <c r="R14" s="14"/>
+      <c r="R14" s="11"/>
       <c r="T14" s="8"/>
     </row>
     <row r="15" spans="3:20">
@@ -3809,15 +3809,15 @@
         <v>21</v>
       </c>
       <c r="H15" s="5"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="11"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="14"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="Q15" s="8"/>
-      <c r="R15" s="14"/>
+      <c r="R15" s="11"/>
       <c r="T15" s="8"/>
     </row>
     <row r="16" spans="3:20">
@@ -3835,7 +3835,7 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="Q16" s="8"/>
-      <c r="R16" s="14"/>
+      <c r="R16" s="11"/>
       <c r="T16" s="8"/>
     </row>
     <row r="17" spans="3:20">
@@ -3855,7 +3855,7 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="Q17" s="8"/>
-      <c r="R17" s="14"/>
+      <c r="R17" s="11"/>
       <c r="T17" s="8"/>
     </row>
     <row r="18" spans="3:20">
@@ -3877,7 +3877,7 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="Q18" s="8"/>
-      <c r="R18" s="14"/>
+      <c r="R18" s="11"/>
       <c r="T18" s="8"/>
     </row>
     <row r="19" spans="3:20">
@@ -3897,7 +3897,7 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="Q19" s="8"/>
-      <c r="R19" s="14"/>
+      <c r="R19" s="11"/>
       <c r="T19" s="8"/>
     </row>
     <row r="20" spans="3:20">
@@ -3915,7 +3915,7 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="Q20" s="8"/>
-      <c r="R20" s="14"/>
+      <c r="R20" s="11"/>
       <c r="T20" s="8"/>
     </row>
     <row r="21" spans="3:20">
@@ -3937,7 +3937,7 @@
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="Q21" s="8"/>
-      <c r="R21" s="14"/>
+      <c r="R21" s="11"/>
       <c r="T21" s="8"/>
     </row>
     <row r="22" spans="3:20">
@@ -3955,7 +3955,7 @@
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="Q22" s="8"/>
-      <c r="R22" s="14"/>
+      <c r="R22" s="11"/>
       <c r="T22" s="8"/>
     </row>
     <row r="23" spans="3:20">
@@ -3977,7 +3977,7 @@
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
       <c r="Q23" s="8"/>
-      <c r="R23" s="14"/>
+      <c r="R23" s="11"/>
       <c r="T23" s="8"/>
     </row>
     <row r="24" spans="3:20">
@@ -3999,7 +3999,7 @@
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
       <c r="Q24" s="8"/>
-      <c r="R24" s="14"/>
+      <c r="R24" s="11"/>
       <c r="T24" s="8"/>
     </row>
     <row r="25" spans="3:20">
@@ -4023,7 +4023,7 @@
         <v>0</v>
       </c>
       <c r="Q25" s="8"/>
-      <c r="R25" s="14"/>
+      <c r="R25" s="11"/>
       <c r="T25" s="8"/>
     </row>
     <row r="26" spans="3:20">
@@ -4032,18 +4032,18 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="12" t="s">
+      <c r="H26" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
       <c r="L26" s="5"/>
       <c r="M26" s="4"/>
       <c r="N26" s="5"/>
       <c r="O26" s="5"/>
       <c r="Q26" s="8"/>
-      <c r="R26" s="14"/>
+      <c r="R26" s="11"/>
       <c r="T26" s="8"/>
     </row>
     <row r="27" spans="3:20">
@@ -4061,7 +4061,7 @@
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
       <c r="Q27" s="8"/>
-      <c r="R27" s="14"/>
+      <c r="R27" s="11"/>
       <c r="T27" s="8"/>
     </row>
     <row r="28" spans="3:20">
@@ -4079,7 +4079,7 @@
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
       <c r="Q28" s="8"/>
-      <c r="R28" s="14"/>
+      <c r="R28" s="11"/>
       <c r="T28" s="8"/>
     </row>
     <row r="29" spans="3:20">
@@ -4097,7 +4097,7 @@
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
       <c r="Q29" s="8"/>
-      <c r="R29" s="14"/>
+      <c r="R29" s="11"/>
       <c r="T29" s="8"/>
     </row>
     <row r="30" spans="3:20">
@@ -4115,7 +4115,7 @@
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="Q30" s="8"/>
-      <c r="R30" s="14"/>
+      <c r="R30" s="11"/>
       <c r="T30" s="8"/>
     </row>
     <row r="31" spans="3:20">
@@ -4133,7 +4133,7 @@
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="Q31" s="8"/>
-      <c r="R31" s="14"/>
+      <c r="R31" s="11"/>
       <c r="T31" s="8"/>
     </row>
     <row r="32" spans="3:20">
@@ -4151,7 +4151,7 @@
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
       <c r="Q32" s="8"/>
-      <c r="R32" s="14"/>
+      <c r="R32" s="11"/>
       <c r="T32" s="8"/>
     </row>
     <row r="33" spans="3:20">
@@ -4171,7 +4171,7 @@
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="Q33" s="8"/>
-      <c r="R33" s="14"/>
+      <c r="R33" s="11"/>
       <c r="T33" s="8"/>
     </row>
     <row r="34" spans="3:20">
@@ -4193,7 +4193,7 @@
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
       <c r="Q34" s="8"/>
-      <c r="R34" s="14"/>
+      <c r="R34" s="11"/>
       <c r="T34" s="8"/>
     </row>
     <row r="35" spans="3:20">
@@ -4217,7 +4217,7 @@
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
       <c r="Q35" s="8"/>
-      <c r="R35" s="14"/>
+      <c r="R35" s="11"/>
       <c r="T35" s="8"/>
     </row>
     <row r="36" spans="3:20">
@@ -4276,9 +4276,9 @@
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
-      <c r="R38" s="15"/>
-      <c r="S38" s="15"/>
-      <c r="T38" s="15"/>
+      <c r="R38" s="9"/>
+      <c r="S38" s="9"/>
+      <c r="T38" s="9"/>
     </row>
     <row r="39" spans="3:20">
       <c r="C39" s="5"/>
@@ -4296,9 +4296,9 @@
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
-      <c r="R39" s="15"/>
-      <c r="S39" s="15"/>
-      <c r="T39" s="15"/>
+      <c r="R39" s="9"/>
+      <c r="S39" s="9"/>
+      <c r="T39" s="9"/>
     </row>
     <row r="40" spans="3:20">
       <c r="C40" s="5" t="s">
@@ -4507,7 +4507,9 @@
         <v>40</v>
       </c>
       <c r="D52" s="5"/>
-      <c r="E52" s="4"/>
+      <c r="E52" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
@@ -4528,7 +4530,9 @@
         <v>20</v>
       </c>
       <c r="F53" s="5"/>
-      <c r="G53" s="4"/>
+      <c r="G53" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
@@ -4543,7 +4547,9 @@
         <v>13</v>
       </c>
       <c r="D54" s="5"/>
-      <c r="E54" s="4"/>
+      <c r="E54" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
@@ -4596,11 +4602,11 @@
     <row r="57" spans="3:15">
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
-      <c r="E57" s="12" t="s">
+      <c r="E57" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
       <c r="H57" s="5"/>
       <c r="I57" s="4"/>
       <c r="J57" s="5"/>
@@ -4664,9 +4670,11 @@
         <v>4</v>
       </c>
       <c r="D61" s="5"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="10"/>
-      <c r="G61" s="11"/>
+      <c r="E61" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F61" s="13"/>
+      <c r="G61" s="14"/>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
@@ -4712,16 +4720,11 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="T28:T31"/>
-    <mergeCell ref="T32:T35"/>
-    <mergeCell ref="R38:T38"/>
-    <mergeCell ref="R39:T39"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="T4:T7"/>
-    <mergeCell ref="T8:T11"/>
-    <mergeCell ref="T12:T15"/>
-    <mergeCell ref="T16:T19"/>
-    <mergeCell ref="T20:T23"/>
+    <mergeCell ref="Q24:Q27"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="C2:O2"/>
     <mergeCell ref="T24:T27"/>
     <mergeCell ref="Q28:Q31"/>
     <mergeCell ref="Q32:Q35"/>
@@ -4738,11 +4741,16 @@
     <mergeCell ref="Q12:Q15"/>
     <mergeCell ref="Q16:Q19"/>
     <mergeCell ref="Q20:Q23"/>
-    <mergeCell ref="Q24:Q27"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="C2:O2"/>
+    <mergeCell ref="T4:T7"/>
+    <mergeCell ref="T8:T11"/>
+    <mergeCell ref="T12:T15"/>
+    <mergeCell ref="T16:T19"/>
+    <mergeCell ref="T20:T23"/>
+    <mergeCell ref="T28:T31"/>
+    <mergeCell ref="T32:T35"/>
+    <mergeCell ref="R38:T38"/>
+    <mergeCell ref="R39:T39"/>
+    <mergeCell ref="E57:G57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>